<commit_message>
New changes with bug fix and first 60 plus stock analysis.
</commit_message>
<xml_diff>
--- a/src/dataframes/input/input_portfolio.xlsx
+++ b/src/dataframes/input/input_portfolio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raman\developer\Configure_VSCode\src\dataframes\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\OptimizeMyPortfolio\src\dataframes\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B24D240-54DA-404C-83AF-DAC63202977B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142A7EC8-7F18-4706-9595-D39C0EB539D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31060" yWindow="2970" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>Stock</t>
   </si>
@@ -45,24 +45,9 @@
     <t>Stock_ID</t>
   </si>
   <si>
-    <t>GOOG</t>
-  </si>
-  <si>
     <t>MSFT</t>
   </si>
   <si>
-    <t>FB</t>
-  </si>
-  <si>
-    <t>AAPL</t>
-  </si>
-  <si>
-    <t>ARKF</t>
-  </si>
-  <si>
-    <t>ENPH</t>
-  </si>
-  <si>
     <t>AMZN</t>
   </si>
   <si>
@@ -72,7 +57,190 @@
     <t>PLTR</t>
   </si>
   <si>
-    <t>RDS-A</t>
+    <t>TM</t>
+  </si>
+  <si>
+    <t>BYD</t>
+  </si>
+  <si>
+    <t>HON</t>
+  </si>
+  <si>
+    <t>RTX</t>
+  </si>
+  <si>
+    <t>LMT</t>
+  </si>
+  <si>
+    <t>2222.SR</t>
+  </si>
+  <si>
+    <t>XOM</t>
+  </si>
+  <si>
+    <t>CVX</t>
+  </si>
+  <si>
+    <t>IBE.MC</t>
+  </si>
+  <si>
+    <t>JPM</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>BAC</t>
+  </si>
+  <si>
+    <t>NESN.SW</t>
+  </si>
+  <si>
+    <t>MCD</t>
+  </si>
+  <si>
+    <t>UL</t>
+  </si>
+  <si>
+    <t>CMG</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>LLY</t>
+  </si>
+  <si>
+    <t>NVO</t>
+  </si>
+  <si>
+    <t>JNJ</t>
+  </si>
+  <si>
+    <t>ABBV</t>
+  </si>
+  <si>
+    <t>PFE</t>
+  </si>
+  <si>
+    <t>VRTX</t>
+  </si>
+  <si>
+    <t>UNP</t>
+  </si>
+  <si>
+    <t>AMT</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>CSX</t>
+  </si>
+  <si>
+    <t>GOO</t>
+  </si>
+  <si>
+    <t>META</t>
+  </si>
+  <si>
+    <t>TCS.NS</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>INFY</t>
+  </si>
+  <si>
+    <t>WIT</t>
+  </si>
+  <si>
+    <t>CTSH</t>
+  </si>
+  <si>
+    <t>CAP.PA</t>
+  </si>
+  <si>
+    <t>NFLX</t>
+  </si>
+  <si>
+    <t>DIS</t>
+  </si>
+  <si>
+    <t>CMCSA</t>
+  </si>
+  <si>
+    <t>SONY</t>
+  </si>
+  <si>
+    <t>SPOT</t>
+  </si>
+  <si>
+    <t>BHP</t>
+  </si>
+  <si>
+    <t>601088.SS</t>
+  </si>
+  <si>
+    <t>RIO</t>
+  </si>
+  <si>
+    <t>SCCO</t>
+  </si>
+  <si>
+    <t>FCX</t>
+  </si>
+  <si>
+    <t>VALE</t>
+  </si>
+  <si>
+    <t>LT.NS</t>
+  </si>
+  <si>
+    <t>DG.PA</t>
+  </si>
+  <si>
+    <t>DHI</t>
+  </si>
+  <si>
+    <t>LEN</t>
+  </si>
+  <si>
+    <t>WMT</t>
+  </si>
+  <si>
+    <t>COST</t>
+  </si>
+  <si>
+    <t>HD</t>
+  </si>
+  <si>
+    <t>BABA</t>
+  </si>
+  <si>
+    <t>MAERSK-B.CO</t>
+  </si>
+  <si>
+    <t>HLAG.DE</t>
+  </si>
+  <si>
+    <t>UBER</t>
+  </si>
+  <si>
+    <t>UPS</t>
+  </si>
+  <si>
+    <t>^GSPC</t>
+  </si>
+  <si>
+    <t>ASML</t>
+  </si>
+  <si>
+    <t>TLT</t>
   </si>
 </sst>
 </file>
@@ -391,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -418,10 +586,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1">
-        <v>606.92999999999995</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -429,10 +597,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="C3" s="1">
-        <v>567.70000000000005</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -440,10 +608,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="C4" s="1">
-        <v>617.34</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -451,10 +619,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
-        <v>214.8</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -465,7 +633,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1">
-        <v>418.56</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -476,7 +644,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1">
-        <v>891.98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -484,10 +652,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1">
-        <v>3451.95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -495,10 +663,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1">
-        <v>4986.22</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -509,7 +677,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1">
-        <v>5934.47</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -517,15 +685,642 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1">
-        <v>25626.400000000001</v>
+      <c r="C12" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C54" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>57</v>
+      </c>
+      <c r="C59" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>60</v>
+      </c>
+      <c r="C62" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>63</v>
+      </c>
+      <c r="C65" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>64</v>
+      </c>
+      <c r="C66" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>31</v>
+      </c>
+      <c r="C67" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" s="1">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C7">
-    <sortCondition descending="1" ref="C2:C7"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:C10">
+    <sortCondition descending="1" ref="C5:C10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>